<commit_message>
A new test case file is created in which all test cases will run together
</commit_message>
<xml_diff>
--- a/TestData/Create_activity.xlsx
+++ b/TestData/Create_activity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mohni\PycharmProjects\cchc_automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB9149F9-F340-4AAF-A3FB-9D07C7B94841}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EC2CB79-67FA-4C04-B55B-3D102D247040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,7 +63,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-409]h:mm\ AM/PM;@"/>
-    <numFmt numFmtId="168" formatCode="mm/dd/yyyy"/>
+    <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -116,7 +116,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -401,7 +401,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>